<commit_message>
linea insert para postgres
</commit_message>
<xml_diff>
--- a/LINKS_GRUPOS.xlsx
+++ b/LINKS_GRUPOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maloa\Documents\CAR\Contrato Abril\Celulas\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CODIGOS\WebScraping MinCiencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D728649-2720-4B0F-8742-4DA4DA1CB8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494495CF-56B1-4A33-B7C9-9967E2A0FAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF10273B-91C6-4F6E-845D-F68A10F95462}"/>
   </bookViews>
@@ -18566,10 +18566,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-[$$-240A]\ * #,##0.0000_-;\-[$$-240A]\ * #,##0.0000_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-240A]\ * #,##0.0000_-;\-[$$-240A]\ * #,##0.0000_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -18652,7 +18652,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -18667,10 +18667,15 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18678,11 +18683,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -18992,7 +18992,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19003,8 +19003,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:B6161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6046" workbookViewId="0">
-      <selection activeCell="I6147" sqref="I6147"/>
+    <sheetView tabSelected="1" topLeftCell="A6039" workbookViewId="0">
+      <selection activeCell="J6062" sqref="J6062"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67421,7 +67421,7 @@
       <c r="A6052">
         <v>6051</v>
       </c>
-      <c r="B6052" t="s">
+      <c r="B6052" s="1" t="s">
         <v>6051</v>
       </c>
     </row>
@@ -68300,6 +68300,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4B4AF80C-5218-4BE7-82BE-AD2E25D089A7}"/>
+    <hyperlink ref="B6052" r:id="rId2" xr:uid="{A169598C-EB5A-488D-BF82-23BFF02279E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -68321,13 +68322,13 @@
   <sheetData>
     <row r="1" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:25" ht="39" x14ac:dyDescent="0.3">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>6162</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>6163</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>6164</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -68343,24 +68344,24 @@
         <v>6171</v>
       </c>
       <c r="K2" s="3"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="S2" s="3"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
     <row r="3" spans="3:25" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
         <v>6166</v>
       </c>
@@ -68374,15 +68375,15 @@
         <v>6172</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
@@ -68395,7 +68396,7 @@
       <c r="D4" s="6">
         <v>265109</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>263061</v>
       </c>
       <c r="F4" s="7">
@@ -68618,7 +68619,7 @@
       <c r="I13" s="7">
         <v>0</v>
       </c>
-      <c r="K13" s="11"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5">
@@ -68642,7 +68643,7 @@
       <c r="I14" s="7">
         <v>0</v>
       </c>
-      <c r="K14" s="11"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5">
@@ -68666,7 +68667,7 @@
       <c r="I15" s="7">
         <v>0</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5">
@@ -68690,7 +68691,7 @@
       <c r="I16" s="7">
         <v>0</v>
       </c>
-      <c r="K16" s="11"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5">
@@ -68714,7 +68715,7 @@
       <c r="I17" s="7">
         <v>0</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="5">
@@ -68738,7 +68739,7 @@
       <c r="I18" s="7">
         <v>0</v>
       </c>
-      <c r="K18" s="11"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="5">
@@ -68877,7 +68878,7 @@
       <c r="I24" s="7">
         <v>0</v>
       </c>
-      <c r="K24" s="11"/>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="5">
@@ -68949,54 +68950,54 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D29" s="10">
-        <f>SUM(D4:D27)</f>
+      <c r="D29" s="8">
+        <f t="shared" ref="D29:I29" si="0">SUM(D4:D27)</f>
         <v>8754461</v>
       </c>
-      <c r="E29" s="10">
-        <f>SUM(E4:E27)</f>
+      <c r="E29" s="8">
+        <f t="shared" si="0"/>
         <v>7460664</v>
       </c>
-      <c r="F29" s="11">
-        <f>SUM(F4:F27)</f>
+      <c r="F29" s="9">
+        <f t="shared" si="0"/>
         <v>470494</v>
       </c>
-      <c r="G29" s="10">
-        <f>SUM(G4:G27)</f>
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
         <v>560</v>
       </c>
-      <c r="H29" s="10">
-        <f>SUM(H4:H27)</f>
+      <c r="H29" s="8">
+        <f t="shared" si="0"/>
         <v>822716</v>
       </c>
-      <c r="I29" s="11">
-        <f>SUM(I4:I27)</f>
+      <c r="I29" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D31" s="10">
-        <f>SUM(D16:D27)</f>
+      <c r="D31" s="8">
+        <f t="shared" ref="D31:I31" si="1">SUM(D16:D27)</f>
         <v>5378990</v>
       </c>
-      <c r="E31" s="10">
-        <f>SUM(E16:E27)</f>
+      <c r="E31" s="8">
+        <f t="shared" si="1"/>
         <v>4371743</v>
       </c>
-      <c r="F31" s="10">
-        <f>SUM(F16:F27)</f>
+      <c r="F31" s="8">
+        <f t="shared" si="1"/>
         <v>301630</v>
       </c>
-      <c r="G31" s="10">
-        <f>SUM(G16:G27)</f>
+      <c r="G31" s="8">
+        <f t="shared" si="1"/>
         <v>416</v>
       </c>
-      <c r="H31" s="10">
-        <f>SUM(H16:H27)</f>
+      <c r="H31" s="8">
+        <f t="shared" si="1"/>
         <v>705185</v>
       </c>
-      <c r="I31" s="10">
-        <f>SUM(I16:I27)</f>
+      <c r="I31" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>